<commit_message>
EPBDS-7372 Trim all String values in cells. For empty values return null. For sequential reading.
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/test/rules/small.xlsx
+++ b/DEV/org.openl.rules/test/rules/small.xlsx
@@ -15,8 +15,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="B18" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>OpenL User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This cell contains spaces only.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Factor</t>
   </si>
@@ -104,6 +138,12 @@
   <si>
     <t>Indent 2</t>
   </si>
+  <si>
+    <t xml:space="preserve">   Trim me!   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                   </t>
+  </si>
 </sst>
 </file>
 
@@ -112,7 +152,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +199,19 @@
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -560,11 +613,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:B16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,9 +689,20 @@
         <v>6</v>
       </c>
     </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
EPBDS-7372 Add formulas support
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/test/rules/small.xlsx
+++ b/DEV/org.openl.rules/test/rules/small.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -61,7 +61,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color theme="0" tint="-0.34998626667073579"/>
+        <color indexed="55"/>
         <rFont val="Franklin Gothic Book"/>
         <family val="2"/>
       </rPr>
@@ -89,17 +89,16 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="0" tint="-0.34998626667073579"/>
+        <color indexed="55"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="0" tint="-0.34998626667073579"/>
+        <color indexed="55"/>
         <rFont val="Franklin Gothic Book"/>
         <family val="2"/>
         <charset val="204"/>
@@ -109,7 +108,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color theme="0" tint="-0.34998626667073579"/>
+        <color indexed="55"/>
         <rFont val="Franklin Gothic Book"/>
         <family val="2"/>
       </rPr>
@@ -118,7 +117,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="0" tint="-0.34998626667073579"/>
+        <color indexed="55"/>
         <rFont val="Franklin Gothic Book"/>
         <family val="2"/>
         <charset val="204"/>
@@ -168,7 +167,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="0" tint="-0.34998626667073579"/>
+      <color indexed="55"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
     </font>
@@ -181,17 +180,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0" tint="-0.34998626667073579"/>
+      <color indexed="55"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0" tint="-0.34998626667073579"/>
+      <color indexed="55"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -199,19 +210,6 @@
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
       <charset val="204"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -223,12 +221,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -236,6 +228,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -258,7 +256,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -268,7 +266,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -278,22 +276,22 @@
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -304,10 +302,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -617,7 +615,7 @@
   <dimension ref="B5:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,7 +655,7 @@
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11">
-        <f>B7 / 2</f>
+        <f>B7/2</f>
         <v>0.75</v>
       </c>
     </row>
@@ -669,13 +667,13 @@
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
-        <f xml:space="preserve"> "Concat" &amp; B5</f>
+        <f>"Concat"&amp;B5</f>
         <v>ConcatValue</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" t="b">
-        <f xml:space="preserve"> 5 &gt; 4</f>
+        <f>5&gt;4</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
EPBDS-7507 Workaround for Shared Formulas in xls files. Fallback to empty style if error is occurred while reading table styles.
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/test/rules/small.xlsx
+++ b/DEV/org.openl.rules/test/rules/small.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="2" r:id="rId1"/>
     <sheet name="Second" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Formulas" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -614,7 +615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -779,4 +780,109 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C12" si="0">B3*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
EPBDS-8798 Fix the bug: failed to load dependent module because of ArrayIndexOutOfBoundsException
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/test/rules/small.xlsx
+++ b/DEV/org.openl.rules/test/rules/small.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ABAD265-FF3A-4BBA-8732-E6C564553133}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="2" r:id="rId1"/>
@@ -12,17 +13,25 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Formulas" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Author</author>
+    <author>Автор</author>
   </authors>
   <commentList>
-    <comment ref="B18" authorId="0">
+    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -51,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Factor</t>
   </si>
@@ -144,11 +153,17 @@
   <si>
     <t xml:space="preserve">                                   </t>
   </si>
+  <si>
+    <t>Meaningful data</t>
+  </si>
+  <si>
+    <t>Last cell</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -314,7 +329,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -322,14 +337,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -367,9 +385,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -402,9 +420,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -437,9 +472,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -612,90 +664,95 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:B18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B5:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B8" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B9" s="7">
         <v>43454</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B10" s="8">
         <v>43455</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B11">
         <f>B7/2</f>
         <v>0.75</v>
       </c>
     </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B12" s="8">
         <f>B10</f>
         <v>43455</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B13" t="str">
         <f>"Concat"&amp;B5</f>
         <v>ConcatValue</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B14" t="b">
         <f>5&gt;4</f>
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B15" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B16" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -706,30 +763,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B4:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:C11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="31.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="11" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="11"/>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
     </row>
-    <row r="6" spans="2:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
@@ -737,7 +794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>2</v>
       </c>
@@ -745,7 +802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" s="5">
         <v>5</v>
       </c>
@@ -753,46 +810,49 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C10" s="13" t="s">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C11" s="13"/>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="13"/>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B4:C5"/>
-    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B10:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B3:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>1</v>
       </c>
@@ -801,7 +861,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>2</v>
       </c>
@@ -810,7 +870,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>3</v>
       </c>
@@ -819,7 +879,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>4</v>
       </c>
@@ -828,7 +888,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>5</v>
       </c>
@@ -837,7 +897,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>6</v>
       </c>
@@ -846,7 +906,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>7</v>
       </c>
@@ -855,7 +915,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>8</v>
       </c>
@@ -864,7 +924,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>9</v>
       </c>
@@ -873,7 +933,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>10</v>
       </c>

</xml_diff>